<commit_message>
Added status display on HDMI output and completed manual
</commit_message>
<xml_diff>
--- a/PCB/V1-7/BusRaider V1.7 BOM.xlsx
+++ b/PCB/V1-7/BusRaider V1.7 BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\RobDev\Projects\Vintage\RC2014\PiBusRaider\PCB\V1-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18492471-A8D0-4085-B487-47D47CBCA309}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6799054-896B-4FE6-8240-0308B500ACA2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32760" windowHeight="14010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="28140" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -144,9 +144,6 @@
     <t>JP1</t>
   </si>
   <si>
-    <t>10K</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
@@ -514,6 +511,9 @@
   </si>
   <si>
     <t>Header strip (male) and socket strip (female) can be broken out from larger pieces such as https://www.amazon.co.uk/SODIAL-2-54mm-Single-Straight-Female-black/dp/B016U9XYBG</t>
+  </si>
+  <si>
+    <t>1K</t>
   </si>
 </sst>
 </file>
@@ -920,8 +920,8 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,28 +980,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5" t="s">
@@ -1013,28 +1013,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5" t="s">
@@ -1046,28 +1046,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5" t="s">
@@ -1085,22 +1085,22 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5" t="s">
@@ -1112,28 +1112,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="H6" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5" t="s">
@@ -1145,28 +1145,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="E7" s="10">
-        <v>1</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>129</v>
-      </c>
       <c r="G7" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="5" t="s">
@@ -1178,28 +1178,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>133</v>
-      </c>
       <c r="D8" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E8" s="10">
         <v>1</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5" t="s">
@@ -1211,13 +1211,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>146</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>147</v>
       </c>
       <c r="E9" s="10">
         <v>1</v>
@@ -1226,13 +1226,13 @@
         <v>5033981892</v>
       </c>
       <c r="G9" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>150</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5" t="s">
@@ -1244,28 +1244,28 @@
         <v>9</v>
       </c>
       <c r="B10" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>101</v>
-      </c>
       <c r="D10" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E10" s="11">
         <v>1</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="J10" s="11"/>
       <c r="K10" s="11" t="s">
@@ -1277,28 +1277,28 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C11" t="s">
         <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5" t="s">
@@ -1313,25 +1313,25 @@
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="G12" t="s">
-        <v>62</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5" t="s">
@@ -1343,7 +1343,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -1355,16 +1355,16 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="I13" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5" t="s">
@@ -1376,28 +1376,28 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D14" t="s">
         <v>139</v>
-      </c>
-      <c r="C14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D14" t="s">
-        <v>140</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5" t="s">
@@ -1409,28 +1409,28 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>38</v>
+        <v>161</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E15" s="10">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" s="4" t="s">
         <v>154</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="E15" s="10">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>155</v>
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5" t="s">
@@ -1442,28 +1442,28 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
         <v>39</v>
       </c>
-      <c r="D16" t="s">
-        <v>40</v>
-      </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="I16" s="16" t="s">
         <v>80</v>
-      </c>
-      <c r="I16" s="16" t="s">
-        <v>81</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5" t="s">
@@ -1475,25 +1475,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="D17" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="E17" s="10">
+        <v>1</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="E17" s="10">
-        <v>1</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="H17" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I17" s="4">
         <v>2889133</v>
@@ -1511,7 +1511,7 @@
         <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D18" t="s">
         <v>24</v>
@@ -1523,13 +1523,13 @@
         <v>23</v>
       </c>
       <c r="G18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5" t="s">
@@ -1553,16 +1553,16 @@
         <v>1</v>
       </c>
       <c r="F19" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="H19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5" t="s">
@@ -1574,28 +1574,28 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>141</v>
+      </c>
+      <c r="C20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" t="s">
         <v>142</v>
-      </c>
-      <c r="C20" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20" t="s">
-        <v>143</v>
       </c>
       <c r="E20">
         <v>3</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5" t="s">
@@ -1607,10 +1607,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" t="s">
         <v>90</v>
-      </c>
-      <c r="C21" t="s">
-        <v>91</v>
       </c>
       <c r="D21" t="s">
         <v>31</v>
@@ -1619,13 +1619,13 @@
         <v>1</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I21" s="4">
         <v>1105963</v>
@@ -1640,10 +1640,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>31</v>
@@ -1652,13 +1652,13 @@
         <v>1</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I22" s="4">
         <v>1105965</v>
@@ -1685,13 +1685,13 @@
         <v>1</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I23" s="4">
         <v>1470786</v>
@@ -1721,10 +1721,10 @@
         <v>35</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I24" s="4">
         <v>9591664</v>
@@ -1739,28 +1739,28 @@
         <v>24</v>
       </c>
       <c r="B25" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="D25" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="E25" s="11">
+        <v>1</v>
+      </c>
+      <c r="F25" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="E25" s="11">
-        <v>1</v>
-      </c>
-      <c r="F25" s="11" t="s">
+      <c r="G25" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="H25" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="I25" s="17" t="s">
         <v>97</v>
-      </c>
-      <c r="I25" s="17" t="s">
-        <v>98</v>
       </c>
       <c r="J25" s="11"/>
       <c r="K25" s="11" t="s">
@@ -1772,10 +1772,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>31</v>
@@ -1784,7 +1784,7 @@
         <v>2</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
@@ -1801,28 +1801,28 @@
         <v>26</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>30</v>
       </c>
       <c r="D27" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="11">
+        <v>1</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G27" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E27" s="11">
-        <v>1</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="G27" s="11" t="s">
+      <c r="H27" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="I27" s="17" t="s">
         <v>104</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="I27" s="17" t="s">
-        <v>105</v>
       </c>
       <c r="J27" s="11"/>
       <c r="K27" s="11" t="s">
@@ -1837,7 +1837,7 @@
         <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D28" t="s">
         <v>26</v>
@@ -1846,13 +1846,13 @@
         <v>4</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I28" s="4">
         <v>1749756</v>
@@ -1867,28 +1867,28 @@
         <v>28</v>
       </c>
       <c r="B29" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" t="s">
         <v>84</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="F29" s="3" t="s">
+      <c r="G29" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I29" s="8" t="s">
         <v>87</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="I29" s="8" t="s">
-        <v>88</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5" t="s">
@@ -1915,13 +1915,13 @@
         <v>27</v>
       </c>
       <c r="G30" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I30" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5" t="s">
@@ -1933,25 +1933,25 @@
         <v>30</v>
       </c>
       <c r="B31" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E31" s="12">
+        <v>1</v>
+      </c>
+      <c r="F31" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="E31" s="12">
-        <v>1</v>
-      </c>
-      <c r="F31" s="12" t="s">
+      <c r="G31" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="G31" s="12" t="s">
+      <c r="H31" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="H31" s="12" t="s">
+      <c r="I31" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="I31" s="8" t="s">
+      <c r="K31" s="12" t="s">
         <v>111</v>
-      </c>
-      <c r="K31" s="12" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1959,30 +1959,30 @@
         <v>31</v>
       </c>
       <c r="B32" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="E32" s="12">
+        <v>1</v>
+      </c>
+      <c r="F32" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="E32" s="12">
-        <v>1</v>
-      </c>
-      <c r="F32" s="12" t="s">
+      <c r="G32" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="G32" s="12" t="s">
-        <v>115</v>
-      </c>
       <c r="H32" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K32" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on pausing at debug start
Now handles multi-line debug commands
Manual updated
</commit_message>
<xml_diff>
--- a/PCB/V1-7/BusRaider V1.7 BOM.xlsx
+++ b/PCB/V1-7/BusRaider V1.7 BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\RobDev\Projects\Vintage\RC2014\PiBusRaider\PCB\V1-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6799054-896B-4FE6-8240-0308B500ACA2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9A34B5-978E-48CB-84E4-11A6598F7063}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="540" windowWidth="28140" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1485" yWindow="1440" windowWidth="28800" windowHeight="19920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -444,9 +444,6 @@
     <t>R1,R4</t>
   </si>
   <si>
-    <t>470R</t>
-  </si>
-  <si>
     <t>AXIAL 3.2x1.8 1/8 WATT</t>
   </si>
   <si>
@@ -514,6 +511,9 @@
   </si>
   <si>
     <t>1K</t>
+  </si>
+  <si>
+    <t>470R or 330R</t>
   </si>
 </sst>
 </file>
@@ -585,7 +585,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -599,10 +599,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -921,7 +918,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,7 +961,7 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -1140,23 +1137,23 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" t="s">
         <v>125</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" t="s">
         <v>126</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" t="s">
         <v>127</v>
       </c>
-      <c r="E7" s="10">
-        <v>1</v>
-      </c>
-      <c r="F7" s="10" t="s">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
         <v>128</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -1173,29 +1170,29 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" t="s">
         <v>131</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" t="s">
         <v>132</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" t="s">
         <v>120</v>
       </c>
-      <c r="E8" s="10">
-        <v>1</v>
-      </c>
-      <c r="F8" s="10" t="s">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
         <v>51</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" t="s">
         <v>43</v>
       </c>
       <c r="I8" s="4" t="s">
@@ -1206,33 +1203,33 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" t="s">
         <v>144</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="D9" t="s">
         <v>145</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="11">
+        <v>5033981892</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="E9" s="10">
-        <v>1</v>
-      </c>
-      <c r="F9" s="14">
-        <v>5033981892</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="4" t="s">
         <v>148</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>149</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5" t="s">
@@ -1243,32 +1240,32 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="E10" s="11">
-        <v>1</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="E10" s="9">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
         <v>51</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" t="s">
         <v>43</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11" t="s">
+      <c r="J10" s="9"/>
+      <c r="K10" s="9" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1376,19 +1373,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="C14" t="s">
         <v>137</v>
       </c>
       <c r="D14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>50</v>
@@ -1397,31 +1394,31 @@
         <v>43</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="E15" s="10">
+        <v>152</v>
+      </c>
+      <c r="D15" t="s">
+        <v>138</v>
+      </c>
+      <c r="E15">
         <v>1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>50</v>
@@ -1430,7 +1427,7 @@
         <v>43</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5" t="s">
@@ -1442,7 +1439,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
@@ -1462,7 +1459,7 @@
       <c r="H16" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="I16" s="16" t="s">
+      <c r="I16" s="13" t="s">
         <v>80</v>
       </c>
       <c r="J16" s="5"/>
@@ -1470,27 +1467,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C17" t="s">
         <v>156</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="D17" t="s">
         <v>157</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="E17" s="10">
-        <v>1</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>159</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>70</v>
@@ -1574,13 +1571,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C20" t="s">
         <v>81</v>
       </c>
       <c r="D20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E20">
         <v>3</v>
@@ -1635,24 +1632,24 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="10">
-        <v>1</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>71</v>
@@ -1738,32 +1735,32 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E25" s="11">
-        <v>1</v>
-      </c>
-      <c r="F25" s="11" t="s">
+      <c r="E25" s="9">
+        <v>1</v>
+      </c>
+      <c r="F25" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="G25" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="I25" s="17" t="s">
+      <c r="I25" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11" t="s">
+      <c r="J25" s="9"/>
+      <c r="K25" s="9" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1771,28 +1768,28 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D26" s="11" t="s">
+      <c r="C26" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="9">
         <v>2</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F26" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
       <c r="I26" s="4">
         <v>1470823</v>
       </c>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11" t="s">
+      <c r="J26" s="9"/>
+      <c r="K26" s="9" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1800,32 +1797,32 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="E27" s="11">
-        <v>1</v>
-      </c>
-      <c r="F27" s="11" t="s">
+      <c r="E27" s="9">
+        <v>1</v>
+      </c>
+      <c r="F27" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G27" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H27" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="I27" s="17" t="s">
+      <c r="I27" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11" t="s">
+      <c r="J27" s="9"/>
+      <c r="K27" s="9" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1866,13 +1863,13 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" t="s">
         <v>83</v>
       </c>
       <c r="C29" t="s">
         <v>84</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" t="s">
         <v>85</v>
       </c>
       <c r="E29">
@@ -1911,7 +1908,7 @@
       <c r="E30">
         <v>1</v>
       </c>
-      <c r="F30" s="13" t="s">
+      <c r="F30" s="10" t="s">
         <v>27</v>
       </c>
       <c r="G30" s="3" t="s">
@@ -1932,25 +1929,25 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="E31" s="12">
-        <v>1</v>
-      </c>
-      <c r="F31" s="12" t="s">
+      <c r="E31" s="9">
+        <v>1</v>
+      </c>
+      <c r="F31" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="G31" s="12" t="s">
+      <c r="G31" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="H31" s="12" t="s">
+      <c r="H31" s="9" t="s">
         <v>109</v>
       </c>
       <c r="I31" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="K31" s="12" t="s">
+      <c r="K31" s="9" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1958,22 +1955,22 @@
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E32" s="12">
-        <v>1</v>
-      </c>
-      <c r="F32" s="12" t="s">
+      <c r="E32" s="9">
+        <v>1</v>
+      </c>
+      <c r="F32" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="G32" s="12" t="s">
+      <c r="G32" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="H32" s="12" t="s">
+      <c r="H32" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="K32" s="12" t="s">
+      <c r="K32" s="9" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1982,7 +1979,7 @@
         <v>128</v>
       </c>
       <c r="B34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes and tidy up
Delay before OTA update
Increased stack size
Added ISR disable/enable to fix uartMaxi problem
</commit_message>
<xml_diff>
--- a/PCB/V1-7/BusRaider V1.7 BOM.xlsx
+++ b/PCB/V1-7/BusRaider V1.7 BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\RobDev\Projects\Vintage\RC2014\PiBusRaider\PCB\V1-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9A34B5-978E-48CB-84E4-11A6598F7063}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF148CA-BFEC-4C66-8DE6-9CC26443DF83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1485" yWindow="1440" windowWidth="28800" windowHeight="19920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="159">
   <si>
     <t>ID</t>
   </si>
@@ -303,27 +302,15 @@
     <t>U14</t>
   </si>
   <si>
-    <t>74HC138 DIL</t>
-  </si>
-  <si>
     <t>U6</t>
   </si>
   <si>
     <t>DIP254P762X420-16</t>
   </si>
   <si>
-    <t>74HC138</t>
-  </si>
-  <si>
     <t>FM</t>
   </si>
   <si>
-    <t>LCSC</t>
-  </si>
-  <si>
-    <t>C86611</t>
-  </si>
-  <si>
     <t>74HCT74N</t>
   </si>
   <si>
@@ -342,9 +329,6 @@
     <t>Nexperia</t>
   </si>
   <si>
-    <t>C6049</t>
-  </si>
-  <si>
     <t>74HCT74</t>
   </si>
   <si>
@@ -514,6 +498,12 @@
   </si>
   <si>
     <t>470R or 330R</t>
+  </si>
+  <si>
+    <t>74HCT138 DIL</t>
+  </si>
+  <si>
+    <t>74HCT138</t>
   </si>
 </sst>
 </file>
@@ -585,7 +575,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -604,7 +594,6 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -918,7 +907,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,13 +966,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1010,13 +999,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1043,19 +1032,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>50</v>
@@ -1064,7 +1053,7 @@
         <v>43</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5" t="s">
@@ -1082,7 +1071,7 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1109,13 +1098,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1142,28 +1131,28 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C7" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="5" t="s">
@@ -1175,13 +1164,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C8" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D8" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1208,13 +1197,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C9" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D9" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -1223,13 +1212,13 @@
         <v>5033981892</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5" t="s">
@@ -1241,13 +1230,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E10" s="9">
         <v>1</v>
@@ -1274,13 +1263,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C11" t="s">
         <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -1310,10 +1299,10 @@
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D12" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -1373,19 +1362,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C14" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D14" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>50</v>
@@ -1394,7 +1383,7 @@
         <v>43</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5" t="s">
@@ -1406,19 +1395,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D15" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>50</v>
@@ -1427,7 +1416,7 @@
         <v>43</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5" t="s">
@@ -1439,7 +1428,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
@@ -1472,22 +1461,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C17" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D17" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>70</v>
@@ -1508,7 +1497,7 @@
         <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D18" t="s">
         <v>24</v>
@@ -1571,13 +1560,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C20" t="s">
         <v>81</v>
       </c>
       <c r="D20" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E20">
         <v>3</v>
@@ -1637,10 +1626,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D22" t="s">
         <v>31</v>
@@ -1649,7 +1638,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>71</v>
@@ -1736,28 +1725,28 @@
         <v>24</v>
       </c>
       <c r="B25" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="D25" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="E25" s="9">
+        <v>1</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G25" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E25" s="9">
-        <v>1</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>95</v>
-      </c>
       <c r="H25" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="I25" s="14" t="s">
-        <v>97</v>
+        <v>70</v>
+      </c>
+      <c r="I25" s="4">
+        <v>1470803</v>
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="9" t="s">
@@ -1769,10 +1758,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>31</v>
@@ -1781,10 +1770,12 @@
         <v>2</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
+      <c r="H26" s="9" t="s">
+        <v>70</v>
+      </c>
       <c r="I26" s="4">
         <v>1470823</v>
       </c>
@@ -1798,28 +1789,28 @@
         <v>26</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>30</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E27" s="9">
         <v>1</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="I27" s="14" t="s">
-        <v>104</v>
+        <v>70</v>
+      </c>
+      <c r="I27" s="4">
+        <v>2463753</v>
       </c>
       <c r="J27" s="9"/>
       <c r="K27" s="9" t="s">
@@ -1930,25 +1921,25 @@
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E31" s="9">
+        <v>1</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="K31" s="9" t="s">
         <v>106</v>
-      </c>
-      <c r="E31" s="9">
-        <v>1</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="K31" s="9" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1956,30 +1947,30 @@
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E32" s="9">
         <v>1</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H32" s="9" t="s">
         <v>67</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B34" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2015,8 +2006,10 @@
     <hyperlink ref="I22" r:id="rId28" tooltip="1105965" display="https://uk.farnell.com/texas-instruments/cd74hct08e/74hct-cmos-74hct08-dip14-5-5v/dp/1105965?st=cd74hct08" xr:uid="{2D279BCB-992E-49D5-ACA8-8EBDBD37D408}"/>
     <hyperlink ref="I15" r:id="rId29" display="https://uk.rs-online.com/web/p/through-hole-fixed-resistors/7077745/" xr:uid="{91D3C579-DB83-44E6-91DC-FBA03F5B49BC}"/>
     <hyperlink ref="I17" r:id="rId30" tooltip="2889133" display="https://uk.farnell.com/vishay/bat85s-tap/diode-schottky-aec-q101-30v-do/dp/2889133?st=bat85" xr:uid="{A58953B0-5C12-4D11-BF34-79E8E8B8C7D3}"/>
+    <hyperlink ref="I25" r:id="rId31" display="https://uk.farnell.com/texas-instruments/sn74hct138n/ic-decoder-demux/dp/1470803" xr:uid="{088E7BD0-5F57-4108-B5F4-A73BE7E8886C}"/>
+    <hyperlink ref="I27" r:id="rId32" tooltip="2463753" display="https://uk.farnell.com/nexperia/74lvc07ad-118/buffer-hex-non-inverting-tssop/dp/2463753?st=74lvc07" xr:uid="{1E322879-091A-494C-856B-698CD984D12D}"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="81" orientation="landscape" r:id="rId31"/>
+  <pageSetup paperSize="9" scale="81" orientation="landscape" r:id="rId33"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed a bug in F2 (immediate mode) keyboard handling
</commit_message>
<xml_diff>
--- a/PCB/V1-7/BusRaider V1.7 BOM.xlsx
+++ b/PCB/V1-7/BusRaider V1.7 BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\RobDev\Projects\Vintage\RC2014\PiBusRaider\PCB\V1-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF148CA-BFEC-4C66-8DE6-9CC26443DF83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93898FB-DA32-408D-94B0-5B023A94B21E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1485" yWindow="1440" windowWidth="28800" windowHeight="19920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15255" yWindow="1365" windowWidth="28800" windowHeight="20265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="173">
   <si>
     <t>ID</t>
   </si>
@@ -443,9 +443,6 @@
     <t>U13,U10</t>
   </si>
   <si>
-    <t>MICRO SD</t>
-  </si>
-  <si>
     <t>J11</t>
   </si>
   <si>
@@ -504,13 +501,58 @@
   </si>
   <si>
     <t>74HCT138</t>
+  </si>
+  <si>
+    <t>MouserPart</t>
+  </si>
+  <si>
+    <t>595-SN74HCT74N</t>
+  </si>
+  <si>
+    <t>MICRO SD SOCKET</t>
+  </si>
+  <si>
+    <t>538-503398-1892</t>
+  </si>
+  <si>
+    <t>78-BAT85S</t>
+  </si>
+  <si>
+    <t>512-BS170</t>
+  </si>
+  <si>
+    <t>859-LTL-4291</t>
+  </si>
+  <si>
+    <t>595-SN74HCT02N</t>
+  </si>
+  <si>
+    <t>595-SN74HCT08N</t>
+  </si>
+  <si>
+    <t>595-SN74HC590AN</t>
+  </si>
+  <si>
+    <t>595-SN74HC595N</t>
+  </si>
+  <si>
+    <t>595-SN74HCT138N</t>
+  </si>
+  <si>
+    <t>771-74LVC07AD-T</t>
+  </si>
+  <si>
+    <t>595-SN74LVC245AN</t>
+  </si>
+  <si>
+    <t>963-JMK212BBJ476MG-T</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -552,6 +594,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF004A85"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -575,7 +623,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -594,6 +642,8 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -907,7 +957,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,7 +1009,9 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1"/>
+      <c r="L1" s="1" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -1197,13 +1249,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" t="s">
         <v>138</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>139</v>
-      </c>
-      <c r="D9" t="s">
-        <v>140</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -1212,17 +1264,20 @@
         <v>5033981892</v>
       </c>
       <c r="G9" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>143</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5" t="s">
         <v>12</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1356,13 +1411,16 @@
       <c r="K13" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="L13" s="15" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C14" t="s">
         <v>132</v>
@@ -1374,7 +1432,7 @@
         <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>50</v>
@@ -1395,10 +1453,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D15" t="s">
         <v>133</v>
@@ -1407,7 +1465,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>50</v>
@@ -1416,7 +1474,7 @@
         <v>43</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5" t="s">
@@ -1428,7 +1486,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
@@ -1455,28 +1513,31 @@
       <c r="K16" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" t="s">
         <v>150</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>151</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>70</v>
@@ -1488,8 +1549,11 @@
       <c r="K17" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1521,8 +1585,11 @@
       <c r="K18" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1554,8 +1621,11 @@
       <c r="K19" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="L19" s="14" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1588,7 +1658,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1620,16 +1690,19 @@
       <c r="K21" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="D22" t="s">
         <v>31</v>
@@ -1638,7 +1711,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>71</v>
@@ -1653,8 +1726,11 @@
       <c r="K22" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" s="14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1686,12 +1762,15 @@
       <c r="K23" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C24" t="s">
@@ -1719,13 +1798,16 @@
       <c r="K24" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="15" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>91</v>
@@ -1737,7 +1819,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G25" s="9" t="s">
         <v>93</v>
@@ -1752,8 +1834,11 @@
       <c r="K25" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1783,8 +1868,11 @@
       <c r="K26" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="15" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1816,8 +1904,11 @@
       <c r="K27" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1849,8 +1940,11 @@
       <c r="K28" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="L28" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1883,7 +1977,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1916,7 +2010,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1942,7 +2036,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1970,7 +2064,7 @@
         <v>123</v>
       </c>
       <c r="B34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -2008,8 +2102,13 @@
     <hyperlink ref="I17" r:id="rId30" tooltip="2889133" display="https://uk.farnell.com/vishay/bat85s-tap/diode-schottky-aec-q101-30v-do/dp/2889133?st=bat85" xr:uid="{A58953B0-5C12-4D11-BF34-79E8E8B8C7D3}"/>
     <hyperlink ref="I25" r:id="rId31" display="https://uk.farnell.com/texas-instruments/sn74hct138n/ic-decoder-demux/dp/1470803" xr:uid="{088E7BD0-5F57-4108-B5F4-A73BE7E8886C}"/>
     <hyperlink ref="I27" r:id="rId32" tooltip="2463753" display="https://uk.farnell.com/nexperia/74lvc07ad-118/buffer-hex-non-inverting-tssop/dp/2463753?st=74lvc07" xr:uid="{1E322879-091A-494C-856B-698CD984D12D}"/>
+    <hyperlink ref="L26" r:id="rId33" display="https://www.mouser.co.uk/ProductDetail/595-SN74HCT74N" xr:uid="{5DB2B185-4538-4EB0-94D7-F9D164976AEE}"/>
+    <hyperlink ref="L9" r:id="rId34" display="https://www.mouser.co.uk/ProductDetail/538-503398-1892" xr:uid="{44ADD77D-75C2-403F-B840-5637CBB15E6B}"/>
+    <hyperlink ref="L16" r:id="rId35" display="https://www.mouser.co.uk/ProductDetail/652-4613X-1LF-10K" xr:uid="{BDF88165-174B-4645-A8E6-5D98DA4D8E2B}"/>
+    <hyperlink ref="L24" r:id="rId36" display="https://www.mouser.co.uk/ProductDetail/595-SN74HC595N" xr:uid="{D2F684B2-EF7E-4A5D-BCB5-5E290EA9927E}"/>
+    <hyperlink ref="L13" r:id="rId37" display="https://www.mouser.co.uk/ProductDetail/963-JMK212BBJ476MG-T" xr:uid="{1545D293-265F-4347-ADF4-3D3D1395A0DA}"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="81" orientation="landscape" r:id="rId33"/>
+  <pageSetup paperSize="9" scale="81" orientation="landscape" r:id="rId38"/>
 </worksheet>
 </file>
</xml_diff>